<commit_message>
12-06-2021 Address page tests
Test for address:
-Address reset to old value after test for address update
-Added test for add new address
-Added test for delete address
-Test plan updated
</commit_message>
<xml_diff>
--- a/Tests/Project.xlsx
+++ b/Tests/Project.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="110">
   <si>
     <t>Test Case</t>
   </si>
@@ -353,7 +353,19 @@
     <t>Verify delete address</t>
   </si>
   <si>
-    <t>No addresses are available. Add a new address</t>
+    <t>Enter new address title in field</t>
+  </si>
+  <si>
+    <t>New address title is visible in field</t>
+  </si>
+  <si>
+    <t>My second address</t>
+  </si>
+  <si>
+    <t>MY SECOND ADDRESS</t>
+  </si>
+  <si>
+    <t>Leva 45</t>
   </si>
 </sst>
 </file>
@@ -511,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -567,6 +579,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1560,7 +1575,7 @@
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,12 +1827,12 @@
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>105</v>
+      <c r="C21" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -1863,7 +1878,7 @@
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,9 +1979,7 @@
       <c r="E8" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="F8" s="22"/>
       <c r="G8" s="24"/>
       <c r="H8" s="13"/>
     </row>
@@ -1981,9 +1994,7 @@
       <c r="E9" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="F9" s="22"/>
       <c r="G9" s="24"/>
       <c r="H9" s="13"/>
     </row>
@@ -2000,9 +2011,7 @@
       <c r="E10" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="F10" s="22"/>
       <c r="G10" s="24"/>
       <c r="H10" s="13"/>
     </row>
@@ -2019,9 +2028,7 @@
       <c r="E11" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="F11" s="22"/>
       <c r="G11" s="24"/>
       <c r="H11" s="13"/>
     </row>
@@ -2038,9 +2045,7 @@
       <c r="E12" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="F12" s="22"/>
       <c r="G12" s="24"/>
       <c r="H12" s="13"/>
     </row>
@@ -2100,11 +2105,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="22"/>
+        <v>105</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>107</v>
+      </c>
       <c r="E16" s="22" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="24"/>
@@ -2114,9 +2121,13 @@
       <c r="B17" s="23">
         <v>10</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="F17" s="22"/>
       <c r="G17" s="24"/>
       <c r="H17" s="13"/>
@@ -2155,8 +2166,8 @@
       <c r="B21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>84</v>
+      <c r="C21" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -2185,7 +2196,7 @@
       <c r="H23" s="5"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F17">
       <formula1>"Not Run ,Pass,Fail,Block"</formula1>
     </dataValidation>
@@ -2202,7 +2213,7 @@
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,9 +2394,13 @@
       <c r="B13" s="23">
         <v>6</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22" t="s">
+        <v>72</v>
+      </c>
       <c r="F13" s="22"/>
       <c r="G13" s="24"/>
       <c r="H13" s="13"/>
@@ -2394,9 +2409,13 @@
       <c r="B14" s="23">
         <v>7</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22" t="s">
+        <v>72</v>
+      </c>
       <c r="F14" s="22"/>
       <c r="G14" s="24"/>
       <c r="H14" s="13"/>
@@ -2405,9 +2424,13 @@
       <c r="B15" s="23">
         <v>8</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="C15" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="22" t="s">
+        <v>75</v>
+      </c>
       <c r="F15" s="22"/>
       <c r="G15" s="24"/>
       <c r="H15" s="13"/>
@@ -2416,9 +2439,15 @@
       <c r="B16" s="23">
         <v>9</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
+      <c r="C16" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="F16" s="22"/>
       <c r="G16" s="24"/>
       <c r="H16" s="13"/>
@@ -2427,9 +2456,13 @@
       <c r="B17" s="23">
         <v>10</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="F17" s="22"/>
       <c r="G17" s="24"/>
       <c r="H17" s="13"/>
@@ -2498,7 +2531,7 @@
       <c r="H23" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"TEST CASE,BUG REPORT"</formula1>
     </dataValidation>

</xml_diff>